<commit_message>
Set up Maven dependency file
</commit_message>
<xml_diff>
--- a/guitar_shack_data.xlsx
+++ b/guitar_shack_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/araisin/Documents/JasonsGuitarShack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69065D48-A0C1-B447-B68A-E64D150508C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1503E55E-C4C9-5B4E-95FF-14222A663DCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33620" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52800" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guitars" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
   <si>
     <t>Make</t>
   </si>
@@ -192,9 +192,6 @@
     <t>No reordering to be done until sold out - i.e. set stock level to trigger alert at 0.</t>
   </si>
   <si>
-    <t>Calculate stock level to trigger alert based on data we have - ????</t>
-  </si>
-  <si>
     <t>Calculate quantity sold per day</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>Reorder level calculated from past sales data</t>
   </si>
   <si>
-    <t xml:space="preserve">GIVEN there exists past sales data for a product WHEN a reorder level is required THEN reorder level is calculated as </t>
-  </si>
-  <si>
     <t>Lead time</t>
   </si>
   <si>
@@ -277,6 +271,24 @@
   </si>
   <si>
     <t>Historical Sales Start Date</t>
+  </si>
+  <si>
+    <t>GIVEN there exists past sales data for a product WHEN a reorder level is required THEN reorder level is calculated as historical sales within the lead time from the same date in the previous year.</t>
+  </si>
+  <si>
+    <t>Reorder level calculated from recent sales data</t>
+  </si>
+  <si>
+    <t>Current Sales Start Date</t>
+  </si>
+  <si>
+    <t>Current Sales End Date</t>
+  </si>
+  <si>
+    <t>Recent sales</t>
+  </si>
+  <si>
+    <t>GIVEN there does not exist past sales data for a product WHEN a reorder level is required THEN reorder level is calculated as recent sales within the lead time from todays date minus lead time.</t>
   </si>
 </sst>
 </file>
@@ -876,7 +888,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -887,7 +899,7 @@
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -898,7 +910,7 @@
         <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -909,7 +921,7 @@
         <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -917,7 +929,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -925,7 +937,7 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1785,10 +1797,10 @@
     </row>
     <row r="6" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -1796,13 +1808,13 @@
         <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>0</v>
@@ -1820,10 +1832,10 @@
         <v>28</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="80" x14ac:dyDescent="0.2">
@@ -1858,7 +1870,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -1866,7 +1878,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>44</v>
@@ -1874,10 +1886,10 @@
     </row>
     <row r="12" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -1885,16 +1897,16 @@
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1915,7 +1927,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1931,10 +1943,10 @@
     </row>
     <row r="17" spans="2:6" ht="64" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="32" x14ac:dyDescent="0.2">
@@ -1942,16 +1954,16 @@
         <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="16" x14ac:dyDescent="0.2">
@@ -1968,7 +1980,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1982,13 +1994,13 @@
   <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
@@ -2008,15 +2020,15 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2027,19 +2039,19 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
         <v>78</v>
       </c>
-      <c r="E7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" t="s">
-        <v>80</v>
-      </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2070,20 +2082,61 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>71</v>
+      <c r="C11" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>811</v>
+      </c>
+      <c r="C13" s="7">
+        <v>44118</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13" s="7">
+        <v>43739</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44118</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
+      </c>
+      <c r="H13">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2091,12 +2144,12 @@
         <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>